<commit_message>
Switch backend to new demo
</commit_message>
<xml_diff>
--- a/excel/demo.xlsx
+++ b/excel/demo.xlsx
@@ -4,28 +4,145 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="23895" windowHeight="12015"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="18720" windowHeight="7740"/>
   </bookViews>
   <sheets>
-    <sheet name="Excesiv" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="array_data_r" comment="data r">Sheet1!$K1:$M1</definedName>
+    <definedName name="array_data_w" comment="data w">Sheet1!$H1:$J1</definedName>
+    <definedName name="array_data_wr" comment="data w r">Sheet1!$N1:$P1</definedName>
+    <definedName name="array_formula_r" comment="formula r">Sheet1!$T1:$V1</definedName>
+    <definedName name="array_formula_w" comment="formula w">Sheet1!$Q1:$S1</definedName>
+    <definedName name="array_formula_wr" comment="formula w r">Sheet1!$W1:$Y1</definedName>
+    <definedName name="array_header_r" comment="header r">Sheet1!$K$2:$M$2</definedName>
+    <definedName name="array_header_w" comment="header w">Sheet1!$H$2:$J$2</definedName>
+    <definedName name="array_header_wr" comment="header w r">Sheet1!$N$2:$P$2</definedName>
+    <definedName name="data_r" comment="data r">Sheet1!$C1</definedName>
+    <definedName name="data_w" comment="data w">Sheet1!$B1</definedName>
+    <definedName name="data_wr" comment="data w r">Sheet1!$D1</definedName>
+    <definedName name="first_row">5</definedName>
+    <definedName name="formula_r" comment="formula r">Sheet1!$F1</definedName>
+    <definedName name="formula_w" comment="formula w">Sheet1!$E1</definedName>
+    <definedName name="formula_wr" comment="formula w r">Sheet1!$G1</definedName>
+    <definedName name="header_r" comment="header r">Sheet1!$C$2</definedName>
+    <definedName name="header_w" comment="header w">Sheet1!$B$2</definedName>
+    <definedName name="header_wr" comment="header w r">Sheet1!$D$2</definedName>
+    <definedName name="id_number" comment="data w">Sheet1!$A1</definedName>
+    <definedName name="type_data_blank" comment="header w r">Sheet1!$X$2</definedName>
+    <definedName name="type_data_boolean" comment="header w r">Sheet1!$V$2</definedName>
+    <definedName name="type_data_date" comment="header w r">Sheet1!$W$2</definedName>
+    <definedName name="type_data_numeric" comment="header w r">Sheet1!$T$2</definedName>
+    <definedName name="type_data_string" comment="header w r">Sheet1!$U$2</definedName>
+    <definedName name="type_formula_blank" comment="header r">Sheet1!$X$3</definedName>
+    <definedName name="type_formula_boolean" comment="header r">Sheet1!$V$3</definedName>
+    <definedName name="type_formula_date" comment="header r">Sheet1!$W$3</definedName>
+    <definedName name="type_formula_error" comment="header r">Sheet1!$Y$3</definedName>
+    <definedName name="type_formula_numeric" comment="header r">Sheet1!$T$3</definedName>
+    <definedName name="type_formula_string" comment="header r">Sheet1!$U$3</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>Response</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Header Read</t>
+  </si>
+  <si>
+    <t>Header Write</t>
+  </si>
+  <si>
+    <t>Header W/R</t>
+  </si>
+  <si>
+    <t>Data Write</t>
+  </si>
+  <si>
+    <t>Data Read</t>
+  </si>
+  <si>
+    <t>Data W/R</t>
+  </si>
+  <si>
+    <t>Formula Write</t>
+  </si>
+  <si>
+    <t>Formula Read</t>
+  </si>
+  <si>
+    <t>Formula W/R</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Array Data Write</t>
+  </si>
+  <si>
+    <t>Array Header Write</t>
+  </si>
+  <si>
+    <t>Array Header Read</t>
+  </si>
+  <si>
+    <t>Array Header W/R</t>
+  </si>
+  <si>
+    <t>Array Data Read</t>
+  </si>
+  <si>
+    <t>Array Data W/R</t>
+  </si>
+  <si>
+    <t>Array Formula Write</t>
+  </si>
+  <si>
+    <t>Array Formula Read</t>
+  </si>
+  <si>
+    <t>Array Formula W/R</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Blank</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General;\-General;&quot;-&quot;"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -35,31 +152,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,18 +182,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -87,21 +213,225 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -391,29 +721,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="11"/>
+    <col min="4" max="4" width="9.140625" style="12"/>
+    <col min="5" max="5" width="9.140625" style="11" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="11"/>
+    <col min="8" max="9" width="9.140625" style="7"/>
+    <col min="10" max="10" width="9.140625" style="12"/>
+    <col min="11" max="12" width="9.140625" style="7"/>
+    <col min="13" max="13" width="9.140625" style="12"/>
+    <col min="14" max="15" width="9.140625" style="7"/>
+    <col min="16" max="16" width="9.140625" style="12"/>
+    <col min="17" max="18" width="9.140625" style="7"/>
+    <col min="19" max="19" width="9.140625" style="12"/>
+    <col min="20" max="21" width="9.140625" style="7"/>
+    <col min="22" max="22" width="9.140625" style="12"/>
+    <col min="23" max="23" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="7"/>
+    <col min="25" max="25" width="9.140625" style="12"/>
+    <col min="26" max="26" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="8"/>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="41"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="44"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="44"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="2"/>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:26">
+      <c r="A2" s="9"/>
+      <c r="B2" s="25">
+        <v>1.6</v>
+      </c>
+      <c r="C2" s="25">
+        <v>2</v>
+      </c>
+      <c r="D2" s="26">
+        <v>1.8</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="27">
+        <v>-0.9</v>
+      </c>
+      <c r="I2" s="28">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="J2" s="26">
+        <v>2.8</v>
+      </c>
+      <c r="K2" s="29">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="L2" s="29">
+        <v>2</v>
+      </c>
+      <c r="M2" s="26">
+        <v>3</v>
+      </c>
+      <c r="N2" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="O2" s="28">
+        <v>2</v>
+      </c>
+      <c r="P2" s="26">
+        <v>-2.1</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="W2" s="37">
+        <v>41128</v>
+      </c>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="39"/>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="23"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="33">
+        <f>-type_data_numeric</f>
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="U3" s="31" t="str">
+        <f>IF(type_data_string="hello", "world", "what?")</f>
+        <v>world</v>
+      </c>
+      <c r="V3" s="31" t="b">
+        <f>NOT(type_data_boolean)</f>
+        <v>0</v>
+      </c>
+      <c r="W3" s="38">
+        <f>type_data_date+7</f>
+        <v>41135</v>
+      </c>
+      <c r="X3" s="31" t="str">
+        <f>IF(type_data_blank&lt;&gt;"", $X$2, "")</f>
+        <v/>
+      </c>
+      <c r="Y3" s="34" t="e">
+        <f>1/$Y$2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="14" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="44"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="41"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" s="44"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:26" s="7" customFormat="1">
+      <c r="A5" s="11">
+        <v>1</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0</v>
+      </c>
+      <c r="C5" s="21">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>-2</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" ref="E5" si="0">data_w*-header_w</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="20">
+        <f t="shared" ref="F5" si="1">data_r*-header_r</f>
+        <v>-2</v>
+      </c>
+      <c r="G5" s="20">
+        <f t="shared" ref="G5" si="2">data_wr*-header_wr</f>
+        <v>3.6</v>
+      </c>
+      <c r="H5" s="5">
+        <v>-2.4</v>
+      </c>
+      <c r="I5" s="5">
+        <v>-1.2</v>
+      </c>
+      <c r="J5" s="6">
+        <v>-1.8</v>
+      </c>
+      <c r="K5" s="17">
+        <v>1</v>
+      </c>
+      <c r="L5" s="17">
+        <v>0</v>
+      </c>
+      <c r="M5" s="18">
+        <v>-1</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>-2.5</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <f t="shared" ref="Q5:S5" ca="1" si="3">OFFSET(array_data_w, ,COLUMN()-COLUMN(array_formula_w), ,1)*-OFFSET(array_header_w, ,COLUMN()-COLUMN(array_formula_w), ,1)</f>
+        <v>-2.16</v>
+      </c>
+      <c r="R5" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>-2.76</v>
+      </c>
+      <c r="S5" s="6">
+        <f t="shared" ca="1" si="3"/>
+        <v>5.04</v>
+      </c>
+      <c r="T5" s="17">
+        <f t="shared" ref="T5:V5" ca="1" si="4">OFFSET(array_data_r, ,COLUMN()-COLUMN(array_formula_r), ,1)*-OFFSET(array_header_r, ,COLUMN()-COLUMN(array_formula_r), ,1)</f>
+        <v>-1</v>
+      </c>
+      <c r="U5" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="W5" s="5">
+        <f t="shared" ref="W5:Y5" ca="1" si="5">OFFSET(array_data_wr, ,COLUMN()-COLUMN(array_formula_wr), ,1)*-OFFSET(array_header_wr, ,COLUMN()-COLUMN(array_formula_wr), ,1)</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="Y5" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B5:Y1006">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>B5&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>